<commit_message>
Story backlog and taskboard spreadsheets
</commit_message>
<xml_diff>
--- a/Story Backlog.xlsx
+++ b/Story Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Google Drive\John's School\Software Engineering\Project 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\PycharmProjects\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>Story ID</t>
   </si>
@@ -95,9 +95,6 @@
     <t>nurse/doctor</t>
   </si>
   <si>
-    <t>it can be saved to the patients chart</t>
-  </si>
-  <si>
     <t>doctor</t>
   </si>
   <si>
@@ -105,6 +102,12 @@
   </si>
   <si>
     <t>enter patient's vitals, prescriptions, and lab tests</t>
+  </si>
+  <si>
+    <t>enter personal information</t>
+  </si>
+  <si>
+    <t>the system can be udpated to view the information</t>
   </si>
 </sst>
 </file>
@@ -570,7 +573,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +686,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -691,10 +694,10 @@
         <v>22</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="5">
@@ -707,18 +710,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="5">
@@ -731,13 +734,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>

</xml_diff>